<commit_message>
Inicio do Excel continua1
</commit_message>
<xml_diff>
--- a/ProjetoTDD/src/test/resources/Principal.xlsx
+++ b/ProjetoTDD/src/test/resources/Principal.xlsx
@@ -3,19 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mafra.romao\Documents\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{00FB3951-50FC-4EA5-969D-97B6F4B297A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{34F09A72-9164-488B-9A79-C166CEEF576D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0861BF03-1F59-48C8-A90A-FE2905DCFAFF}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="20760" windowHeight="11820" xr2:uid="{0861BF03-1F59-48C8-A90A-FE2905DCFAFF}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,6 +26,26 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>preencheDadosUsuarioTesteCase</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>MafraMano</t>
+  </si>
+  <si>
+    <t>4Jes</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -379,12 +395,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61E856CD-4D57-4853-A409-47292FF7290A}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="40.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>